<commit_message>
tuning hyperparams for genetic algo
</commit_message>
<xml_diff>
--- a/report/6A.xlsx
+++ b/report/6A.xlsx
@@ -460,27 +460,27 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Sinh_T05</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Van_T03</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The_T11</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tin_T00</t>
+          <t>CN_T10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The_T11</t>
+          <t>Sinh_T05</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tin_T00</t>
+          <t>Toan_T00</t>
         </is>
       </c>
     </row>
@@ -490,32 +490,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Toan_T00</t>
+          <t>Dia_T07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Anh_T04</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ly_T01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Anh_T04</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Van_T03</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Su_T06</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Ly_T01</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CN_T10</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Toan_T00</t>
+          <t>The_T11</t>
         </is>
       </c>
     </row>
@@ -525,22 +525,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Toan_T00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tin_T00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Ly_T01</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dia_T07</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Anh_T04</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Toan_T00</t>
+          <t>The_T11</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ly_T01</t>
+          <t>Tin_T00</t>
         </is>
       </c>
     </row>
@@ -560,32 +560,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Van_T03</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Hoa_T02</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Toan_T00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hoa_T02</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>GDCD_T08</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sinh_T05</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Toan_T00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Van_T03</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Anh_T04</t>
+          <t>Su_T06</t>
         </is>
       </c>
     </row>
@@ -595,21 +595,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Ly_T01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Hoa_T02</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hoa_T02</t>
+          <t>Toan_T00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Sinh_T05</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>